<commit_message>
refactor: 5 documents added to retrieval, tranform query removes verbs
</commit_message>
<xml_diff>
--- a/static/Links.xlsx
+++ b/static/Links.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$125</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="167">
   <si>
     <t>Links</t>
   </si>
@@ -278,6 +281,243 @@
   </si>
   <si>
     <t>https://isdunyasi.etu.edu.tr/</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/bilgisayar-muhendisligi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/biyomedikal-muhendisligi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/elektrik-elektronik-muhendisligi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/endustri-muhendisligi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/makine-muhendisligi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/malzeme-bilimi-ve-nanoteknoloji-muh</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/mekatronik-muhendisligi-yandal-programi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/yapay-zeka-muhendisligi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/iktisat</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/isletme</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/siyaset-bilimi-ve-uluslararasi-iliskiler</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/uluslararasi-girisimcilik</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/endustriyel-tasarim</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/gorsel-iletisim-tasarimi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/ic-mimarlik-ve-cevre-tasarimi</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/mimarlik</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/sanat-ve-tasarim</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/hukuk</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/ingiliz-dili-ve-edebiyati</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/matematik</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/psikoloji</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/tarih</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/turk-dili-ve-edebiyati</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/bolum/yabanci-diller-bolumu</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/enstitu/saglik-bilimleri-enstitusu</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/enstitu/sosyal-bilimler-enstitusu</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/tr/enstitu/fen-bilimleri-enstitusu</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/sharer/sharer.php?u=https://www.etu.edu.tr/tr/sayfa/mevzuat&amp;t=Mevzuat</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/shareArticle?mini=true&amp;url=https://www.etu.edu.tr/tr/sayfa/mevzuat&amp;title=Mevzuat&amp;summary=Mevzuat&amp;source=https://www.etu.edu.tr</t>
+  </si>
+  <si>
+    <t>https://twitter.com/intent/tweet?source=https://www.etu.edu.tr/tr/sayfa/mevzuat&amp;text=Mevzuat%20https://goo.gl/OL5ZFe&amp;via=tobbetum</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/editor_images/mevzuat.jpg</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/MevzuatMetin/1.5.2547.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2019/02/08/024e5b616e83775137645eee2c5e8988.pdf</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=7.5.9768&amp;MevzuatIliski=0&amp;sourceXmlSearch=vak%C4%B1f%20y%C3%BCksek%C3%B6%C4%9Fretim</t>
+  </si>
+  <si>
+    <t>https://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=7.5.28996&amp;MevzuatIliski=0&amp;sourceXmlSearch=kalite</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=7.5.13948&amp;MevzuatIliski=0&amp;sourceXmlSearch=%C3%A7ift%20anadal</t>
+  </si>
+  <si>
+    <t>https://www.resmigazete.gov.tr/eskiler/2020/06/20200613-5.htm</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=7.5.8315&amp;MevzuatIliski=0&amp;sourceXmlSearch=meslek</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=7.5.21475&amp;MevzuatIliski=0&amp;sourceXmlSearch=YABANCI%20D%C4%B0L</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=7.5.21510&amp;MevzuatIliski=0&amp;sourceXmlSearch=lisans%C3%BCst%C3%BC</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.6767&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.15287&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.20459&amp;MevzuatIliski=0&amp;sourceXmlSearch</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.8039&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.9564&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.12008&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.13754&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.13907&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.15668&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.17281&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.17282&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.22767&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>http://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.24793&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2019/11/26/a98296c41a24139258e5a903bb6bcd2e.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mevzuat.gov.tr/mevzuat?MevzuatNo=39354&amp;MevzuatTur=8&amp;MevzuatTertip=5</t>
+  </si>
+  <si>
+    <t>https://www.mevzuat.gov.tr/Metin.Aspx?MevzuatKod=8.5.34217&amp;MevzuatIliski=0&amp;sourceXmlSearch=</t>
+  </si>
+  <si>
+    <t>https://www.mevzuat.gov.tr/mevzuat?MevzuatNo=38992&amp;MevzuatTur=8&amp;MevzuatTertip=5</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/sayfa/akademik-personel-atama-ve-yukseltme-usul-ve-esaslari</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/09/06/55b3e1728fb87e7fc221e76f0ff2f65c.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2022/08/24/b808273300f61dae3d83149e3184e67e.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2022/04/01/7a6a6fac58b7a91c50a342bddf446668.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2021/09/28/ac4c0f9f48d7e309b12df6abe5f6de03.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2022/04/29/e4a91d8a9e617c5a7024e31a94bf5e30.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2022/06/21/3eb70a18b5317745498a04da5fc290a6.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2023/01/16/c26ed9f31ec61fdbf969bcf14c1a5482.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/07/13/cc78483737d01b2fff3a99858d78f5ca.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/07/13/ab1a55e4a6eb099986f4834fc8bb7e3a.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2023/01/27/dd2d62eec99fe4668fea6f4e53ecca3d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2021/02/03/185aafcba43c8fc133fb7a714af5b259.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/08/24/f90889693628cf27f674cf4d7b0b2f14.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/08/16/ce3e595cfd3f1734d84b258c76d4e4a6.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2021/09/28/74cd79a31b7184bb5aca80c563ef7f43.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/04/19/c8dfe01a8f99af5da67e4636e07cd807.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2017/04/19/ced70e1323507919c80d34bbc35b6fd9.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2018/07/12/f76bf2a66921c030bbb79e237de561ee.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2021/09/28/646a1745649a8675acd54592eba8fddb.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2018/05/08/38eba8f69b8a0770b5fb7bb3797fc880.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2023/01/19/d211153c734beb559a5efedeb6cf3194.pdf</t>
+  </si>
+  <si>
+    <t>https://www.etu.edu.tr/files/dosyalar/2021/03/17/552de35f0414765d5b921f490b022b69.pdf</t>
   </si>
 </sst>
 </file>
@@ -285,12 +525,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,9 +552,112 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,63 +671,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -396,26 +692,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -426,35 +707,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -465,91 +717,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,25 +861,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,61 +897,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,17 +911,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,46 +944,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -756,18 +982,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -777,134 +1029,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -912,6 +1164,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,16 +1487,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:A122"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="87.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="20.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1262,9 +1520,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>_xlfn.UNIQUE(A2:A204)</f>
+        <v>https://www.etu.edu.tr/en</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -1312,7 +1574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" hidden="1" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1332,7 +1594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" hidden="1" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1377,7 +1639,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" hidden="1" spans="1:1">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -1387,7 +1649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" hidden="1" spans="1:1">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1407,7 +1669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" hidden="1" spans="1:1">
       <c r="A34" s="2" t="s">
         <v>26</v>
       </c>
@@ -1427,7 +1689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" hidden="1" spans="1:1">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
@@ -1457,7 +1719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" hidden="1" spans="1:1">
       <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
@@ -1467,7 +1729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" hidden="1" spans="1:1">
       <c r="A46" s="2" t="s">
         <v>33</v>
       </c>
@@ -1492,7 +1754,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" hidden="1" spans="1:1">
       <c r="A51" s="2" t="s">
         <v>11</v>
       </c>
@@ -1527,7 +1789,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" hidden="1" spans="1:1">
       <c r="A58" s="2" t="s">
         <v>44</v>
       </c>
@@ -1542,7 +1804,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" hidden="1" spans="1:1">
       <c r="A61" s="2" t="s">
         <v>11</v>
       </c>
@@ -1552,7 +1814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" hidden="1" spans="1:1">
       <c r="A63" s="2" t="s">
         <v>45</v>
       </c>
@@ -1562,17 +1824,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" hidden="1" spans="1:1">
       <c r="A65" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" hidden="1" spans="1:1">
       <c r="A66" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" hidden="1" spans="1:1">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
@@ -1592,7 +1854,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" hidden="1" spans="1:1">
       <c r="A71" s="2" t="s">
         <v>24</v>
       </c>
@@ -1677,7 +1939,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" hidden="1" spans="1:1">
       <c r="A88" s="2" t="s">
         <v>23</v>
       </c>
@@ -1717,7 +1979,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" hidden="1" spans="1:1">
       <c r="A96" s="2" t="s">
         <v>13</v>
       </c>
@@ -1767,82 +2029,82 @@
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" hidden="1" spans="1:1">
       <c r="A106" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" hidden="1" spans="1:1">
       <c r="A107" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" hidden="1" spans="1:1">
       <c r="A108" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" hidden="1" spans="1:1">
       <c r="A109" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" hidden="1" spans="1:1">
       <c r="A110" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" hidden="1" spans="1:1">
       <c r="A111" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" hidden="1" spans="1:1">
       <c r="A112" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" hidden="1" spans="1:1">
       <c r="A113" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" hidden="1" spans="1:1">
       <c r="A114" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" hidden="1" spans="1:1">
       <c r="A115" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" hidden="1" spans="1:1">
       <c r="A116" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" hidden="1" spans="1:1">
       <c r="A117" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" hidden="1" spans="1:1">
       <c r="A118" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" hidden="1" spans="1:1">
       <c r="A119" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" hidden="1" spans="1:1">
       <c r="A120" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" hidden="1" spans="1:1">
       <c r="A121" s="2" t="s">
         <v>1</v>
       </c>
@@ -1850,6 +2112,416 @@
     <row r="122" spans="1:1">
       <c r="A122" s="2" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="123" hidden="1" spans="1:1">
+      <c r="A123" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" hidden="1" spans="1:1">
+      <c r="A124" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="125" hidden="1" spans="1:1">
+      <c r="A125" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="143" ht="18" spans="1:1">
+      <c r="A143" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="154" ht="27.6" spans="1:1">
+      <c r="A154" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="155" ht="27.6" spans="1:1">
+      <c r="A155" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="159" ht="27.6" spans="1:1">
+      <c r="A159" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="160" ht="27.6" spans="1:1">
+      <c r="A160" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="161" ht="27.6" spans="1:1">
+      <c r="A161" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="163" ht="27.6" spans="1:1">
+      <c r="A163" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="164" ht="27.6" spans="1:1">
+      <c r="A164" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="165" ht="27.6" spans="1:1">
+      <c r="A165" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>